<commit_message>
added draft of hybrid figure
</commit_message>
<xml_diff>
--- a/4_aviation/energy_density/data/data.xlsx
+++ b/4_aviation/energy_density/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelweinold/github/phd_publication_figures/4_aviation/energy_density/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31F4197-F5A0-B14F-BC2D-C550A6D49CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E21D0F6-CC69-B747-B63D-AD7D78A1CAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{B845ADF3-7D47-1941-B9F3-1A771EDB3806}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{B845ADF3-7D47-1941-B9F3-1A771EDB3806}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Density Fuels" sheetId="3" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -480,6 +480,12 @@
   </si>
   <si>
     <t>give a pack factor energy density loss of 25%</t>
+  </si>
+  <si>
+    <t>some new battery</t>
+  </si>
+  <si>
+    <t>https://news.yahoo.com/nasa-incredible-solid-state-battery-130000645.html</t>
   </si>
 </sst>
 </file>
@@ -558,10 +564,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1403,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C730CE0-2479-7E43-807E-3BF76EDF0063}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1568,10 +1570,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3DF2F86-30C6-2246-A264-173C0F9F5AEF}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1683,6 +1685,14 @@
       </c>
       <c r="D8" s="2" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>